<commit_message>
I suck at Coding
</commit_message>
<xml_diff>
--- a/Record.xlsx
+++ b/Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill Li\Desktop\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E67B48B-0879-4B5B-816B-EBA4DC08FD3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C33A5D-14F2-4592-B2D7-D4BB211247C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6143333D-C90C-4E83-8A8F-03E6D88CE1AA}"/>
   </bookViews>
@@ -1465,7 +1465,7 @@
   <dimension ref="A2:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="K5" s="16">
         <f>COUNT(K11:K25)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="31"/>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="K6" s="17">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="14"/>
       <c r="M6" s="33"/>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="K8" s="47">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L8" s="47">
         <f t="shared" si="9"/>
@@ -1920,7 +1920,7 @@
       </c>
       <c r="C11" s="70">
         <f>SUM(G5:M5)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="109" t="s">
         <v>20</v>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="C12" s="71">
         <f>SUM(G6:M6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="110"/>
       <c r="E12" s="101"/>
@@ -2017,7 +2017,9 @@
       <c r="J13" s="19">
         <v>485</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="19">
+        <v>1030</v>
+      </c>
       <c r="L13" s="4"/>
       <c r="M13" s="40"/>
       <c r="N13" s="11"/>
@@ -2036,7 +2038,7 @@
       </c>
       <c r="C14" s="73">
         <f>SUM(G8:M8)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="110"/>
       <c r="E14" s="101"/>
@@ -2410,7 +2412,9 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="1"/>
+      <c r="K27" s="25">
+        <v>951</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="40"/>
       <c r="N27" s="11"/>

</xml_diff>